<commit_message>
Layout + Download Excel
</commit_message>
<xml_diff>
--- a/datasets/DataBreaches_initialAttackVectors(2).xlsx
+++ b/datasets/DataBreaches_initialAttackVectors(2).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timkossmann/Desktop/Uni/Semester 6/Data Storytelling/storytelling/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF29A068-2084-1B46-B4AD-20DBC3D03073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42FA4680-E937-BF4D-901B-3FECEB7D7071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{2285D1E5-7DD9-4EE3-89A7-1FA6076E39D5}"/>
   </bookViews>
@@ -81,6 +81,9 @@
     <t>Social Engineering</t>
   </si>
   <si>
+    <t>Kompromittierung von Geschäfts-E-Mails</t>
+  </si>
+  <si>
     <t>Systemfehler</t>
   </si>
   <si>
@@ -118,9 +121,6 @@
   </si>
   <si>
     <t>Fehler</t>
-  </si>
-  <si>
-    <t>Kompromittierung\nvon\nGeschäfts-E-Mails</t>
   </si>
 </sst>
 </file>
@@ -501,19 +501,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
         <v>27</v>
-      </c>
-      <c r="E1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -543,7 +543,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -560,7 +560,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5">
         <v>5</v>
@@ -577,7 +577,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6">
         <v>6</v>
@@ -594,7 +594,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7">
         <v>8</v>
@@ -611,7 +611,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B8">
         <v>9</v>
@@ -628,7 +628,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9">
         <v>14</v>
@@ -645,7 +645,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B10">
         <v>15</v>
@@ -662,7 +662,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B11">
         <v>17</v>
@@ -679,7 +679,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B12">
         <v>20</v>

</xml_diff>